<commit_message>
Update Excel files for new format
</commit_message>
<xml_diff>
--- a/conflictMatrices/conflict-matrix-v0.1.xlsx
+++ b/conflictMatrices/conflict-matrix-v0.1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerjan\Workshop\TrafficLightController\conflictMatrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706D2B15-785D-4B68-8999-A36B5AA80A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59369F9-2019-4A98-A9D4-B0AD7633020A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-2400" windowWidth="25440" windowHeight="15990" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
+    <workbookView xWindow="12915" yWindow="240" windowWidth="25770" windowHeight="20505" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Setup" sheetId="2" r:id="rId1"/>
+    <sheet name="ConflictMatrix" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -432,10 +433,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCF9752-FF37-4260-BA3B-FE4874A85D41}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="B1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B482FAD3-CCB3-9E48-B087-47D1B142F0B2}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>